<commit_message>
Fixed bug on overtime approval
</commit_message>
<xml_diff>
--- a/rpt/overtime.xlsx
+++ b/rpt/overtime.xlsx
@@ -286,7 +286,7 @@
       <c r="J3" s="1" t="inlineStr"/>
       <c r="K3" s="1" t="inlineStr"/>
       <c r="L3" s="4">
-        <v>44364.90393518517</v>
+        <v>44548.629016203806</v>
       </c>
       <c r="M3" s="5" t="inlineStr"/>
       <c r="N3" s="5" t="inlineStr"/>
@@ -349,7 +349,7 @@
       <c r="B6" s="6" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">MANDAL, MV LEBERTY PAMOLERAS</t>
+            <t xml:space="preserve">CELEBRE, EDGAR TUALLA</t>
           </r>
         </is>
       </c>
@@ -418,21 +418,21 @@
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="4">
-        <v>44313.0</v>
+        <v>44544.0</v>
       </c>
       <c r="F8" s="5" t="inlineStr"/>
       <c r="G8" s="5" t="inlineStr"/>
       <c r="H8" s="5" t="inlineStr"/>
       <c r="I8" s="9">
-        <v>25569.815972222015</v>
+        <v>25569.65416666679</v>
       </c>
       <c r="J8" s="9">
-        <v>25569.524305555504</v>
+        <v>25569.866666666698</v>
       </c>
       <c r="K8" s="5" t="inlineStr"/>
       <c r="L8" s="5" t="inlineStr"/>
       <c r="M8" s="8" t="n">
-        <v>7.0</v>
+        <v>5.6</v>
       </c>
       <c r="N8" s="5" t="inlineStr"/>
       <c r="O8" s="5" t="inlineStr"/>
@@ -444,25 +444,25 @@
       <c r="B9" s="1" t="inlineStr"/>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
-      <c r="E9" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F9" s="5" t="inlineStr"/>
-      <c r="G9" s="5" t="inlineStr"/>
-      <c r="H9" s="5" t="inlineStr"/>
-      <c r="I9" s="9">
-        <v>25569.824305555783</v>
-      </c>
-      <c r="J9" s="9">
-        <v>25569.824305555783</v>
+      <c r="E9" s="1" t="inlineStr"/>
+      <c r="F9" s="1" t="inlineStr"/>
+      <c r="G9" s="1" t="inlineStr"/>
+      <c r="H9" s="1" t="inlineStr"/>
+      <c r="I9" s="1" t="inlineStr"/>
+      <c r="J9" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Emp Total Hrs</t>
+          </r>
+        </is>
       </c>
       <c r="K9" s="5" t="inlineStr"/>
       <c r="L9" s="5" t="inlineStr"/>
-      <c r="M9" s="8" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="N9" s="5" t="inlineStr"/>
-      <c r="O9" s="5" t="inlineStr"/>
+      <c r="M9" s="10" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="N9" s="11" t="inlineStr"/>
+      <c r="O9" s="11" t="inlineStr"/>
       <c r="P9" s="1" t="inlineStr"/>
       <c r="Q9" s="1" t="inlineStr"/>
     </row>
@@ -471,79 +471,81 @@
       <c r="B10" s="1" t="inlineStr"/>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
-      <c r="E10" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F10" s="5" t="inlineStr"/>
-      <c r="G10" s="5" t="inlineStr"/>
-      <c r="H10" s="5" t="inlineStr"/>
-      <c r="I10" s="9">
-        <v>25569.75</v>
-      </c>
-      <c r="J10" s="9">
-        <v>25569.79166666651</v>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" s="1" t="inlineStr"/>
+      <c r="G10" s="1" t="inlineStr"/>
+      <c r="H10" s="1" t="inlineStr"/>
+      <c r="I10" s="1" t="inlineStr"/>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Dep Total Hrs</t>
+          </r>
+        </is>
       </c>
       <c r="K10" s="5" t="inlineStr"/>
       <c r="L10" s="5" t="inlineStr"/>
-      <c r="M10" s="8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="N10" s="5" t="inlineStr"/>
-      <c r="O10" s="5" t="inlineStr"/>
+      <c r="M10" s="10" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="N10" s="11" t="inlineStr"/>
+      <c r="O10" s="11" t="inlineStr"/>
       <c r="P10" s="1" t="inlineStr"/>
       <c r="Q10" s="1" t="inlineStr"/>
     </row>
     <row r="11" customHeight="1" ht="20">
       <c r="A11" s="1" t="inlineStr"/>
-      <c r="B11" s="1" t="inlineStr"/>
-      <c r="C11" s="1" t="inlineStr"/>
-      <c r="D11" s="1" t="inlineStr"/>
-      <c r="E11" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F11" s="5" t="inlineStr"/>
-      <c r="G11" s="5" t="inlineStr"/>
-      <c r="H11" s="5" t="inlineStr"/>
-      <c r="I11" s="9">
-        <v>25569.824305555783</v>
-      </c>
-      <c r="J11" s="9">
-        <v>25569.824305555783</v>
-      </c>
-      <c r="K11" s="5" t="inlineStr"/>
-      <c r="L11" s="5" t="inlineStr"/>
-      <c r="M11" s="8" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="N11" s="5" t="inlineStr"/>
-      <c r="O11" s="5" t="inlineStr"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">150</t>
+          </r>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">MIS</t>
+          </r>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="1" t="inlineStr"/>
+      <c r="G11" s="1" t="inlineStr"/>
+      <c r="H11" s="1" t="inlineStr"/>
+      <c r="I11" s="1" t="inlineStr"/>
+      <c r="J11" s="1" t="inlineStr"/>
+      <c r="K11" s="1" t="inlineStr"/>
+      <c r="L11" s="1" t="inlineStr"/>
+      <c r="M11" s="1" t="inlineStr"/>
+      <c r="N11" s="1" t="inlineStr"/>
+      <c r="O11" s="1" t="inlineStr"/>
       <c r="P11" s="1" t="inlineStr"/>
       <c r="Q11" s="1" t="inlineStr"/>
     </row>
     <row r="12" customHeight="1" ht="20">
       <c r="A12" s="1" t="inlineStr"/>
-      <c r="B12" s="1" t="inlineStr"/>
-      <c r="C12" s="1" t="inlineStr"/>
-      <c r="D12" s="1" t="inlineStr"/>
-      <c r="E12" s="1" t="inlineStr"/>
-      <c r="F12" s="1" t="inlineStr"/>
-      <c r="G12" s="1" t="inlineStr"/>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ASINAS, MARLON DURAN</t>
+          </r>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
       <c r="H12" s="1" t="inlineStr"/>
       <c r="I12" s="1" t="inlineStr"/>
-      <c r="J12" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Emp Total Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="K12" s="5" t="inlineStr"/>
-      <c r="L12" s="5" t="inlineStr"/>
-      <c r="M12" s="10" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="N12" s="11" t="inlineStr"/>
-      <c r="O12" s="11" t="inlineStr"/>
+      <c r="J12" s="1" t="inlineStr"/>
+      <c r="K12" s="1" t="inlineStr"/>
+      <c r="L12" s="1" t="inlineStr"/>
+      <c r="M12" s="1" t="inlineStr"/>
+      <c r="N12" s="1" t="inlineStr"/>
+      <c r="O12" s="1" t="inlineStr"/>
       <c r="P12" s="1" t="inlineStr"/>
       <c r="Q12" s="1" t="inlineStr"/>
     </row>
@@ -552,81 +554,95 @@
       <c r="B13" s="1" t="inlineStr"/>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
-      <c r="E13" s="1" t="inlineStr"/>
-      <c r="F13" s="1" t="inlineStr"/>
-      <c r="G13" s="1" t="inlineStr"/>
-      <c r="H13" s="1" t="inlineStr"/>
-      <c r="I13" s="1" t="inlineStr"/>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Date Filed</t>
+          </r>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr"/>
+      <c r="G13" s="5" t="inlineStr"/>
+      <c r="H13" s="5" t="inlineStr"/>
+      <c r="I13" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Start Time</t>
+          </r>
+        </is>
+      </c>
       <c r="J13" s="8" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">Dep Total Hrs</t>
+            <t xml:space="preserve">End Time</t>
           </r>
         </is>
       </c>
       <c r="K13" s="5" t="inlineStr"/>
       <c r="L13" s="5" t="inlineStr"/>
-      <c r="M13" s="10" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="N13" s="11" t="inlineStr"/>
-      <c r="O13" s="11" t="inlineStr"/>
+      <c r="M13" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Hrs</t>
+          </r>
+        </is>
+      </c>
+      <c r="N13" s="5" t="inlineStr"/>
+      <c r="O13" s="5" t="inlineStr"/>
       <c r="P13" s="1" t="inlineStr"/>
       <c r="Q13" s="1" t="inlineStr"/>
     </row>
     <row r="14" customHeight="1" ht="20">
       <c r="A14" s="1" t="inlineStr"/>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">150</t>
-          </r>
-        </is>
-      </c>
-      <c r="C14" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">MIS</t>
-          </r>
-        </is>
-      </c>
-      <c r="D14" s="7" t="inlineStr"/>
-      <c r="E14" s="7" t="inlineStr"/>
-      <c r="F14" s="1" t="inlineStr"/>
-      <c r="G14" s="1" t="inlineStr"/>
-      <c r="H14" s="1" t="inlineStr"/>
-      <c r="I14" s="1" t="inlineStr"/>
-      <c r="J14" s="1" t="inlineStr"/>
-      <c r="K14" s="1" t="inlineStr"/>
-      <c r="L14" s="1" t="inlineStr"/>
-      <c r="M14" s="1" t="inlineStr"/>
-      <c r="N14" s="1" t="inlineStr"/>
-      <c r="O14" s="1" t="inlineStr"/>
+      <c r="B14" s="1" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr"/>
+      <c r="D14" s="1" t="inlineStr"/>
+      <c r="E14" s="4">
+        <v>44541.0</v>
+      </c>
+      <c r="F14" s="5" t="inlineStr"/>
+      <c r="G14" s="5" t="inlineStr"/>
+      <c r="H14" s="5" t="inlineStr"/>
+      <c r="I14" s="9">
+        <v>25569.25</v>
+      </c>
+      <c r="J14" s="9">
+        <v>25569.75</v>
+      </c>
+      <c r="K14" s="5" t="inlineStr"/>
+      <c r="L14" s="5" t="inlineStr"/>
+      <c r="M14" s="8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="N14" s="5" t="inlineStr"/>
+      <c r="O14" s="5" t="inlineStr"/>
       <c r="P14" s="1" t="inlineStr"/>
       <c r="Q14" s="1" t="inlineStr"/>
     </row>
     <row r="15" customHeight="1" ht="20">
       <c r="A15" s="1" t="inlineStr"/>
-      <c r="B15" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">ABAWAG, REINHARD CIRE ESCOBAR</t>
-          </r>
-        </is>
-      </c>
-      <c r="C15" s="7" t="inlineStr"/>
-      <c r="D15" s="7" t="inlineStr"/>
-      <c r="E15" s="7" t="inlineStr"/>
-      <c r="F15" s="7" t="inlineStr"/>
-      <c r="G15" s="7" t="inlineStr"/>
-      <c r="H15" s="1" t="inlineStr"/>
-      <c r="I15" s="1" t="inlineStr"/>
-      <c r="J15" s="1" t="inlineStr"/>
-      <c r="K15" s="1" t="inlineStr"/>
-      <c r="L15" s="1" t="inlineStr"/>
-      <c r="M15" s="1" t="inlineStr"/>
-      <c r="N15" s="1" t="inlineStr"/>
-      <c r="O15" s="1" t="inlineStr"/>
+      <c r="B15" s="1" t="inlineStr"/>
+      <c r="C15" s="1" t="inlineStr"/>
+      <c r="D15" s="1" t="inlineStr"/>
+      <c r="E15" s="4">
+        <v>44541.0</v>
+      </c>
+      <c r="F15" s="5" t="inlineStr"/>
+      <c r="G15" s="5" t="inlineStr"/>
+      <c r="H15" s="5" t="inlineStr"/>
+      <c r="I15" s="9">
+        <v>25569.25</v>
+      </c>
+      <c r="J15" s="9">
+        <v>25569.5</v>
+      </c>
+      <c r="K15" s="5" t="inlineStr"/>
+      <c r="L15" s="5" t="inlineStr"/>
+      <c r="M15" s="8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="N15" s="5" t="inlineStr"/>
+      <c r="O15" s="5" t="inlineStr"/>
       <c r="P15" s="1" t="inlineStr"/>
       <c r="Q15" s="1" t="inlineStr"/>
     </row>
@@ -635,68 +651,50 @@
       <c r="B16" s="1" t="inlineStr"/>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr"/>
-      <c r="E16" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Date Filed</t>
-          </r>
-        </is>
-      </c>
-      <c r="F16" s="5" t="inlineStr"/>
-      <c r="G16" s="5" t="inlineStr"/>
-      <c r="H16" s="5" t="inlineStr"/>
-      <c r="I16" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Start Time</t>
-          </r>
-        </is>
-      </c>
+      <c r="E16" s="1" t="inlineStr"/>
+      <c r="F16" s="1" t="inlineStr"/>
+      <c r="G16" s="1" t="inlineStr"/>
+      <c r="H16" s="1" t="inlineStr"/>
+      <c r="I16" s="1" t="inlineStr"/>
       <c r="J16" s="8" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">End Time</t>
+            <t xml:space="preserve">Emp Total Hrs</t>
           </r>
         </is>
       </c>
       <c r="K16" s="5" t="inlineStr"/>
       <c r="L16" s="5" t="inlineStr"/>
-      <c r="M16" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="N16" s="5" t="inlineStr"/>
-      <c r="O16" s="5" t="inlineStr"/>
+      <c r="M16" s="10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="N16" s="11" t="inlineStr"/>
+      <c r="O16" s="11" t="inlineStr"/>
       <c r="P16" s="1" t="inlineStr"/>
       <c r="Q16" s="1" t="inlineStr"/>
     </row>
     <row r="17" customHeight="1" ht="20">
       <c r="A17" s="1" t="inlineStr"/>
-      <c r="B17" s="1" t="inlineStr"/>
-      <c r="C17" s="1" t="inlineStr"/>
-      <c r="D17" s="1" t="inlineStr"/>
-      <c r="E17" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F17" s="5" t="inlineStr"/>
-      <c r="G17" s="5" t="inlineStr"/>
-      <c r="H17" s="5" t="inlineStr"/>
-      <c r="I17" s="9">
-        <v>25569.827083333395</v>
-      </c>
-      <c r="J17" s="9">
-        <v>25569.827083333395</v>
-      </c>
-      <c r="K17" s="5" t="inlineStr"/>
-      <c r="L17" s="5" t="inlineStr"/>
-      <c r="M17" s="8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N17" s="5" t="inlineStr"/>
-      <c r="O17" s="5" t="inlineStr"/>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ABAWAG, REINHARD CIRE ESCOBAR</t>
+          </r>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr"/>
+      <c r="D17" s="7" t="inlineStr"/>
+      <c r="E17" s="7" t="inlineStr"/>
+      <c r="F17" s="7" t="inlineStr"/>
+      <c r="G17" s="7" t="inlineStr"/>
+      <c r="H17" s="1" t="inlineStr"/>
+      <c r="I17" s="1" t="inlineStr"/>
+      <c r="J17" s="1" t="inlineStr"/>
+      <c r="K17" s="1" t="inlineStr"/>
+      <c r="L17" s="1" t="inlineStr"/>
+      <c r="M17" s="1" t="inlineStr"/>
+      <c r="N17" s="1" t="inlineStr"/>
+      <c r="O17" s="1" t="inlineStr"/>
       <c r="P17" s="1" t="inlineStr"/>
       <c r="Q17" s="1" t="inlineStr"/>
     </row>
@@ -705,22 +703,38 @@
       <c r="B18" s="1" t="inlineStr"/>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr"/>
-      <c r="E18" s="4">
-        <v>44313.0</v>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Date Filed</t>
+          </r>
+        </is>
       </c>
       <c r="F18" s="5" t="inlineStr"/>
       <c r="G18" s="5" t="inlineStr"/>
       <c r="H18" s="5" t="inlineStr"/>
-      <c r="I18" s="9">
-        <v>25569.825000000186</v>
-      </c>
-      <c r="J18" s="9">
-        <v>25569.825000000186</v>
+      <c r="I18" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Start Time</t>
+          </r>
+        </is>
+      </c>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">End Time</t>
+          </r>
+        </is>
       </c>
       <c r="K18" s="5" t="inlineStr"/>
       <c r="L18" s="5" t="inlineStr"/>
-      <c r="M18" s="8" t="n">
-        <v>72.0</v>
+      <c r="M18" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Hrs</t>
+          </r>
+        </is>
       </c>
       <c r="N18" s="5" t="inlineStr"/>
       <c r="O18" s="5" t="inlineStr"/>
@@ -733,21 +747,21 @@
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="4">
-        <v>44309.0</v>
+        <v>44541.0</v>
       </c>
       <c r="F19" s="5" t="inlineStr"/>
       <c r="G19" s="5" t="inlineStr"/>
       <c r="H19" s="5" t="inlineStr"/>
       <c r="I19" s="9">
-        <v>25569.837499999907</v>
+        <v>25569.25</v>
       </c>
       <c r="J19" s="9">
-        <v>25569.837499999907</v>
+        <v>25569.75</v>
       </c>
       <c r="K19" s="5" t="inlineStr"/>
       <c r="L19" s="5" t="inlineStr"/>
       <c r="M19" s="8" t="n">
-        <v>24.0</v>
+        <v>12.0</v>
       </c>
       <c r="N19" s="5" t="inlineStr"/>
       <c r="O19" s="5" t="inlineStr"/>
@@ -760,21 +774,21 @@
       <c r="C20" s="1" t="inlineStr"/>
       <c r="D20" s="1" t="inlineStr"/>
       <c r="E20" s="4">
-        <v>44313.0</v>
+        <v>44541.0</v>
       </c>
       <c r="F20" s="5" t="inlineStr"/>
       <c r="G20" s="5" t="inlineStr"/>
       <c r="H20" s="5" t="inlineStr"/>
       <c r="I20" s="9">
-        <v>25569.815972222015</v>
+        <v>25569.25</v>
       </c>
       <c r="J20" s="9">
-        <v>25569.524305555504</v>
+        <v>25569.75</v>
       </c>
       <c r="K20" s="5" t="inlineStr"/>
       <c r="L20" s="5" t="inlineStr"/>
       <c r="M20" s="8" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="N20" s="5" t="inlineStr"/>
       <c r="O20" s="5" t="inlineStr"/>
@@ -787,21 +801,21 @@
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="4">
-        <v>44313.0</v>
+        <v>44547.0</v>
       </c>
       <c r="F21" s="5" t="inlineStr"/>
       <c r="G21" s="5" t="inlineStr"/>
       <c r="H21" s="5" t="inlineStr"/>
       <c r="I21" s="9">
-        <v>25569.81458333321</v>
+        <v>25569.899999999907</v>
       </c>
       <c r="J21" s="9">
-        <v>25569.522916666698</v>
+        <v>25569.649999999907</v>
       </c>
       <c r="K21" s="5" t="inlineStr"/>
       <c r="L21" s="5" t="inlineStr"/>
       <c r="M21" s="8" t="n">
-        <v>7.0</v>
+        <v>42.0</v>
       </c>
       <c r="N21" s="5" t="inlineStr"/>
       <c r="O21" s="5" t="inlineStr"/>
@@ -813,25 +827,25 @@
       <c r="B22" s="1" t="inlineStr"/>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr"/>
-      <c r="E22" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F22" s="5" t="inlineStr"/>
-      <c r="G22" s="5" t="inlineStr"/>
-      <c r="H22" s="5" t="inlineStr"/>
-      <c r="I22" s="9">
-        <v>25569.809722222388</v>
-      </c>
-      <c r="J22" s="9">
-        <v>25569.309722222388</v>
+      <c r="E22" s="1" t="inlineStr"/>
+      <c r="F22" s="1" t="inlineStr"/>
+      <c r="G22" s="1" t="inlineStr"/>
+      <c r="H22" s="1" t="inlineStr"/>
+      <c r="I22" s="1" t="inlineStr"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Emp Total Hrs</t>
+          </r>
+        </is>
       </c>
       <c r="K22" s="5" t="inlineStr"/>
       <c r="L22" s="5" t="inlineStr"/>
-      <c r="M22" s="8" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="N22" s="5" t="inlineStr"/>
-      <c r="O22" s="5" t="inlineStr"/>
+      <c r="M22" s="10" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="N22" s="11" t="inlineStr"/>
+      <c r="O22" s="11" t="inlineStr"/>
       <c r="P22" s="1" t="inlineStr"/>
       <c r="Q22" s="1" t="inlineStr"/>
     </row>
@@ -848,14 +862,14 @@
       <c r="J23" s="8" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">Emp Total Hrs</t>
+            <t xml:space="preserve">Dep Total Hrs</t>
           </r>
         </is>
       </c>
       <c r="K23" s="5" t="inlineStr"/>
       <c r="L23" s="5" t="inlineStr"/>
       <c r="M23" s="10" t="n">
-        <v>122.0</v>
+        <v>84.0</v>
       </c>
       <c r="N23" s="11" t="inlineStr"/>
       <c r="O23" s="11" t="inlineStr"/>
@@ -864,51 +878,49 @@
     </row>
     <row r="24" customHeight="1" ht="20">
       <c r="A24" s="1" t="inlineStr"/>
-      <c r="B24" s="1" t="inlineStr"/>
-      <c r="C24" s="1" t="inlineStr"/>
-      <c r="D24" s="1" t="inlineStr"/>
-      <c r="E24" s="1" t="inlineStr"/>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">700</t>
+          </r>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">ISO</t>
+          </r>
+        </is>
+      </c>
+      <c r="D24" s="7" t="inlineStr"/>
+      <c r="E24" s="7" t="inlineStr"/>
       <c r="F24" s="1" t="inlineStr"/>
       <c r="G24" s="1" t="inlineStr"/>
       <c r="H24" s="1" t="inlineStr"/>
       <c r="I24" s="1" t="inlineStr"/>
-      <c r="J24" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Dep Total Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="K24" s="5" t="inlineStr"/>
-      <c r="L24" s="5" t="inlineStr"/>
-      <c r="M24" s="10" t="n">
-        <v>122.0</v>
-      </c>
-      <c r="N24" s="11" t="inlineStr"/>
-      <c r="O24" s="11" t="inlineStr"/>
+      <c r="J24" s="1" t="inlineStr"/>
+      <c r="K24" s="1" t="inlineStr"/>
+      <c r="L24" s="1" t="inlineStr"/>
+      <c r="M24" s="1" t="inlineStr"/>
+      <c r="N24" s="1" t="inlineStr"/>
+      <c r="O24" s="1" t="inlineStr"/>
       <c r="P24" s="1" t="inlineStr"/>
       <c r="Q24" s="1" t="inlineStr"/>
     </row>
     <row r="25" customHeight="1" ht="20">
       <c r="A25" s="1" t="inlineStr"/>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">600</t>
-          </r>
-        </is>
-      </c>
-      <c r="C25" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">AUDIT</t>
-          </r>
-        </is>
-      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">MANARIN, JEFFEL KURT NAN</t>
+          </r>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr"/>
       <c r="D25" s="7" t="inlineStr"/>
       <c r="E25" s="7" t="inlineStr"/>
-      <c r="F25" s="1" t="inlineStr"/>
-      <c r="G25" s="1" t="inlineStr"/>
+      <c r="F25" s="7" t="inlineStr"/>
+      <c r="G25" s="7" t="inlineStr"/>
       <c r="H25" s="1" t="inlineStr"/>
       <c r="I25" s="1" t="inlineStr"/>
       <c r="J25" s="1" t="inlineStr"/>
@@ -922,26 +934,44 @@
     </row>
     <row r="26" customHeight="1" ht="20">
       <c r="A26" s="1" t="inlineStr"/>
-      <c r="B26" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">COMIA, SHEBA SALUDES</t>
-          </r>
-        </is>
-      </c>
-      <c r="C26" s="7" t="inlineStr"/>
-      <c r="D26" s="7" t="inlineStr"/>
-      <c r="E26" s="7" t="inlineStr"/>
-      <c r="F26" s="7" t="inlineStr"/>
-      <c r="G26" s="7" t="inlineStr"/>
-      <c r="H26" s="1" t="inlineStr"/>
-      <c r="I26" s="1" t="inlineStr"/>
-      <c r="J26" s="1" t="inlineStr"/>
-      <c r="K26" s="1" t="inlineStr"/>
-      <c r="L26" s="1" t="inlineStr"/>
-      <c r="M26" s="1" t="inlineStr"/>
-      <c r="N26" s="1" t="inlineStr"/>
-      <c r="O26" s="1" t="inlineStr"/>
+      <c r="B26" s="1" t="inlineStr"/>
+      <c r="C26" s="1" t="inlineStr"/>
+      <c r="D26" s="1" t="inlineStr"/>
+      <c r="E26" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Date Filed</t>
+          </r>
+        </is>
+      </c>
+      <c r="F26" s="5" t="inlineStr"/>
+      <c r="G26" s="5" t="inlineStr"/>
+      <c r="H26" s="5" t="inlineStr"/>
+      <c r="I26" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Start Time</t>
+          </r>
+        </is>
+      </c>
+      <c r="J26" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">End Time</t>
+          </r>
+        </is>
+      </c>
+      <c r="K26" s="5" t="inlineStr"/>
+      <c r="L26" s="5" t="inlineStr"/>
+      <c r="M26" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Hrs</t>
+          </r>
+        </is>
+      </c>
+      <c r="N26" s="5" t="inlineStr"/>
+      <c r="O26" s="5" t="inlineStr"/>
       <c r="P26" s="1" t="inlineStr"/>
       <c r="Q26" s="1" t="inlineStr"/>
     </row>
@@ -950,38 +980,22 @@
       <c r="B27" s="1" t="inlineStr"/>
       <c r="C27" s="1" t="inlineStr"/>
       <c r="D27" s="1" t="inlineStr"/>
-      <c r="E27" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Date Filed</t>
-          </r>
-        </is>
+      <c r="E27" s="4">
+        <v>44544.0</v>
       </c>
       <c r="F27" s="5" t="inlineStr"/>
       <c r="G27" s="5" t="inlineStr"/>
       <c r="H27" s="5" t="inlineStr"/>
-      <c r="I27" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Start Time</t>
-          </r>
-        </is>
-      </c>
-      <c r="J27" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">End Time</t>
-          </r>
-        </is>
+      <c r="I27" s="9">
+        <v>25569.649305555504</v>
+      </c>
+      <c r="J27" s="9">
+        <v>25569.649305555504</v>
       </c>
       <c r="K27" s="5" t="inlineStr"/>
       <c r="L27" s="5" t="inlineStr"/>
-      <c r="M27" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Hrs</t>
-          </r>
-        </is>
+      <c r="M27" s="8" t="n">
+        <v>72.0</v>
       </c>
       <c r="N27" s="5" t="inlineStr"/>
       <c r="O27" s="5" t="inlineStr"/>
@@ -993,25 +1007,25 @@
       <c r="B28" s="1" t="inlineStr"/>
       <c r="C28" s="1" t="inlineStr"/>
       <c r="D28" s="1" t="inlineStr"/>
-      <c r="E28" s="4">
-        <v>44310.0</v>
-      </c>
-      <c r="F28" s="5" t="inlineStr"/>
-      <c r="G28" s="5" t="inlineStr"/>
-      <c r="H28" s="5" t="inlineStr"/>
-      <c r="I28" s="9">
-        <v>25569.5784722222</v>
-      </c>
-      <c r="J28" s="9">
-        <v>25569.5784722222</v>
+      <c r="E28" s="1" t="inlineStr"/>
+      <c r="F28" s="1" t="inlineStr"/>
+      <c r="G28" s="1" t="inlineStr"/>
+      <c r="H28" s="1" t="inlineStr"/>
+      <c r="I28" s="1" t="inlineStr"/>
+      <c r="J28" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Emp Total Hrs</t>
+          </r>
+        </is>
       </c>
       <c r="K28" s="5" t="inlineStr"/>
       <c r="L28" s="5" t="inlineStr"/>
-      <c r="M28" s="8" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="N28" s="5" t="inlineStr"/>
-      <c r="O28" s="5" t="inlineStr"/>
+      <c r="M28" s="10" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="N28" s="11" t="inlineStr"/>
+      <c r="O28" s="11" t="inlineStr"/>
       <c r="P28" s="1" t="inlineStr"/>
       <c r="Q28" s="1" t="inlineStr"/>
     </row>
@@ -1028,34 +1042,28 @@
       <c r="J29" s="8" t="inlineStr">
         <is>
           <r>
-            <t xml:space="preserve">Emp Total Hrs</t>
+            <t xml:space="preserve">Dep Total Hrs</t>
           </r>
         </is>
       </c>
       <c r="K29" s="5" t="inlineStr"/>
       <c r="L29" s="5" t="inlineStr"/>
       <c r="M29" s="10" t="n">
-        <v>48.0</v>
+        <v>72.0</v>
       </c>
       <c r="N29" s="11" t="inlineStr"/>
       <c r="O29" s="11" t="inlineStr"/>
       <c r="P29" s="1" t="inlineStr"/>
       <c r="Q29" s="1" t="inlineStr"/>
     </row>
-    <row r="30" customHeight="1" ht="20">
+    <row r="30" customHeight="1" ht="182">
       <c r="A30" s="1" t="inlineStr"/>
-      <c r="B30" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">SAQUIBAL, ARIES VANN RETUYA</t>
-          </r>
-        </is>
-      </c>
-      <c r="C30" s="7" t="inlineStr"/>
-      <c r="D30" s="7" t="inlineStr"/>
-      <c r="E30" s="7" t="inlineStr"/>
-      <c r="F30" s="7" t="inlineStr"/>
-      <c r="G30" s="7" t="inlineStr"/>
+      <c r="B30" s="1" t="inlineStr"/>
+      <c r="C30" s="1" t="inlineStr"/>
+      <c r="D30" s="1" t="inlineStr"/>
+      <c r="E30" s="1" t="inlineStr"/>
+      <c r="F30" s="1" t="inlineStr"/>
+      <c r="G30" s="1" t="inlineStr"/>
       <c r="H30" s="1" t="inlineStr"/>
       <c r="I30" s="1" t="inlineStr"/>
       <c r="J30" s="1" t="inlineStr"/>
@@ -1072,41 +1080,29 @@
       <c r="B31" s="1" t="inlineStr"/>
       <c r="C31" s="1" t="inlineStr"/>
       <c r="D31" s="1" t="inlineStr"/>
-      <c r="E31" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Date Filed</t>
-          </r>
-        </is>
-      </c>
-      <c r="F31" s="5" t="inlineStr"/>
-      <c r="G31" s="5" t="inlineStr"/>
-      <c r="H31" s="5" t="inlineStr"/>
-      <c r="I31" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Start Time</t>
-          </r>
-        </is>
-      </c>
-      <c r="J31" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">End Time</t>
-          </r>
-        </is>
-      </c>
-      <c r="K31" s="5" t="inlineStr"/>
+      <c r="E31" s="1" t="inlineStr"/>
+      <c r="F31" s="1" t="inlineStr"/>
+      <c r="G31" s="1" t="inlineStr"/>
+      <c r="H31" s="1" t="inlineStr"/>
+      <c r="I31" s="1" t="inlineStr"/>
+      <c r="J31" s="1" t="inlineStr"/>
+      <c r="K31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Page 1 of</t>
+          </r>
+        </is>
+      </c>
       <c r="L31" s="5" t="inlineStr"/>
-      <c r="M31" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="N31" s="5" t="inlineStr"/>
-      <c r="O31" s="5" t="inlineStr"/>
+      <c r="M31" s="5" t="inlineStr"/>
+      <c r="N31" s="6" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve"> 1</t>
+          </r>
+        </is>
+      </c>
+      <c r="O31" s="1" t="inlineStr"/>
       <c r="P31" s="1" t="inlineStr"/>
       <c r="Q31" s="1" t="inlineStr"/>
     </row>
@@ -1115,150 +1111,19 @@
       <c r="B32" s="1" t="inlineStr"/>
       <c r="C32" s="1" t="inlineStr"/>
       <c r="D32" s="1" t="inlineStr"/>
-      <c r="E32" s="4">
-        <v>44313.0</v>
-      </c>
-      <c r="F32" s="5" t="inlineStr"/>
-      <c r="G32" s="5" t="inlineStr"/>
-      <c r="H32" s="5" t="inlineStr"/>
-      <c r="I32" s="9">
-        <v>25569.83402777789</v>
-      </c>
-      <c r="J32" s="9">
-        <v>25569.83402777789</v>
-      </c>
-      <c r="K32" s="5" t="inlineStr"/>
-      <c r="L32" s="5" t="inlineStr"/>
-      <c r="M32" s="8" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="N32" s="5" t="inlineStr"/>
-      <c r="O32" s="5" t="inlineStr"/>
+      <c r="E32" s="1" t="inlineStr"/>
+      <c r="F32" s="1" t="inlineStr"/>
+      <c r="G32" s="1" t="inlineStr"/>
+      <c r="H32" s="1" t="inlineStr"/>
+      <c r="I32" s="1" t="inlineStr"/>
+      <c r="J32" s="1" t="inlineStr"/>
+      <c r="K32" s="1" t="inlineStr"/>
+      <c r="L32" s="1" t="inlineStr"/>
+      <c r="M32" s="1" t="inlineStr"/>
+      <c r="N32" s="1" t="inlineStr"/>
+      <c r="O32" s="1" t="inlineStr"/>
       <c r="P32" s="1" t="inlineStr"/>
       <c r="Q32" s="1" t="inlineStr"/>
-    </row>
-    <row r="33" customHeight="1" ht="20">
-      <c r="A33" s="1" t="inlineStr"/>
-      <c r="B33" s="1" t="inlineStr"/>
-      <c r="C33" s="1" t="inlineStr"/>
-      <c r="D33" s="1" t="inlineStr"/>
-      <c r="E33" s="1" t="inlineStr"/>
-      <c r="F33" s="1" t="inlineStr"/>
-      <c r="G33" s="1" t="inlineStr"/>
-      <c r="H33" s="1" t="inlineStr"/>
-      <c r="I33" s="1" t="inlineStr"/>
-      <c r="J33" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Emp Total Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="K33" s="5" t="inlineStr"/>
-      <c r="L33" s="5" t="inlineStr"/>
-      <c r="M33" s="10" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="N33" s="11" t="inlineStr"/>
-      <c r="O33" s="11" t="inlineStr"/>
-      <c r="P33" s="1" t="inlineStr"/>
-      <c r="Q33" s="1" t="inlineStr"/>
-    </row>
-    <row r="34" customHeight="1" ht="20">
-      <c r="A34" s="1" t="inlineStr"/>
-      <c r="B34" s="1" t="inlineStr"/>
-      <c r="C34" s="1" t="inlineStr"/>
-      <c r="D34" s="1" t="inlineStr"/>
-      <c r="E34" s="1" t="inlineStr"/>
-      <c r="F34" s="1" t="inlineStr"/>
-      <c r="G34" s="1" t="inlineStr"/>
-      <c r="H34" s="1" t="inlineStr"/>
-      <c r="I34" s="1" t="inlineStr"/>
-      <c r="J34" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Dep Total Hrs</t>
-          </r>
-        </is>
-      </c>
-      <c r="K34" s="5" t="inlineStr"/>
-      <c r="L34" s="5" t="inlineStr"/>
-      <c r="M34" s="10" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="N34" s="11" t="inlineStr"/>
-      <c r="O34" s="11" t="inlineStr"/>
-      <c r="P34" s="1" t="inlineStr"/>
-      <c r="Q34" s="1" t="inlineStr"/>
-    </row>
-    <row r="35" customHeight="1" ht="82">
-      <c r="A35" s="1" t="inlineStr"/>
-      <c r="B35" s="1" t="inlineStr"/>
-      <c r="C35" s="1" t="inlineStr"/>
-      <c r="D35" s="1" t="inlineStr"/>
-      <c r="E35" s="1" t="inlineStr"/>
-      <c r="F35" s="1" t="inlineStr"/>
-      <c r="G35" s="1" t="inlineStr"/>
-      <c r="H35" s="1" t="inlineStr"/>
-      <c r="I35" s="1" t="inlineStr"/>
-      <c r="J35" s="1" t="inlineStr"/>
-      <c r="K35" s="1" t="inlineStr"/>
-      <c r="L35" s="1" t="inlineStr"/>
-      <c r="M35" s="1" t="inlineStr"/>
-      <c r="N35" s="1" t="inlineStr"/>
-      <c r="O35" s="1" t="inlineStr"/>
-      <c r="P35" s="1" t="inlineStr"/>
-      <c r="Q35" s="1" t="inlineStr"/>
-    </row>
-    <row r="36" customHeight="1" ht="20">
-      <c r="A36" s="1" t="inlineStr"/>
-      <c r="B36" s="1" t="inlineStr"/>
-      <c r="C36" s="1" t="inlineStr"/>
-      <c r="D36" s="1" t="inlineStr"/>
-      <c r="E36" s="1" t="inlineStr"/>
-      <c r="F36" s="1" t="inlineStr"/>
-      <c r="G36" s="1" t="inlineStr"/>
-      <c r="H36" s="1" t="inlineStr"/>
-      <c r="I36" s="1" t="inlineStr"/>
-      <c r="J36" s="1" t="inlineStr"/>
-      <c r="K36" s="8" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve">Page 1 of</t>
-          </r>
-        </is>
-      </c>
-      <c r="L36" s="5" t="inlineStr"/>
-      <c r="M36" s="5" t="inlineStr"/>
-      <c r="N36" s="6" t="inlineStr">
-        <is>
-          <r>
-            <t xml:space="preserve"> 1</t>
-          </r>
-        </is>
-      </c>
-      <c r="O36" s="1" t="inlineStr"/>
-      <c r="P36" s="1" t="inlineStr"/>
-      <c r="Q36" s="1" t="inlineStr"/>
-    </row>
-    <row r="37" customHeight="1" ht="20">
-      <c r="A37" s="1" t="inlineStr"/>
-      <c r="B37" s="1" t="inlineStr"/>
-      <c r="C37" s="1" t="inlineStr"/>
-      <c r="D37" s="1" t="inlineStr"/>
-      <c r="E37" s="1" t="inlineStr"/>
-      <c r="F37" s="1" t="inlineStr"/>
-      <c r="G37" s="1" t="inlineStr"/>
-      <c r="H37" s="1" t="inlineStr"/>
-      <c r="I37" s="1" t="inlineStr"/>
-      <c r="J37" s="1" t="inlineStr"/>
-      <c r="K37" s="1" t="inlineStr"/>
-      <c r="L37" s="1" t="inlineStr"/>
-      <c r="M37" s="1" t="inlineStr"/>
-      <c r="N37" s="1" t="inlineStr"/>
-      <c r="O37" s="1" t="inlineStr"/>
-      <c r="P37" s="1" t="inlineStr"/>
-      <c r="Q37" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -1273,27 +1138,24 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="M8:O8"/>
-    <mergeCell ref="E9:H9"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:O9"/>
-    <mergeCell ref="E10:H10"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="M10:O10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="E13:H13"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M13:O13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M15:O15"/>
     <mergeCell ref="J16:L16"/>
     <mergeCell ref="M16:O16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="B17:G17"/>
     <mergeCell ref="E18:H18"/>
     <mergeCell ref="J18:L18"/>
     <mergeCell ref="M18:O18"/>
@@ -1306,35 +1168,23 @@
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="M21:O21"/>
-    <mergeCell ref="E22:H22"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="M22:O22"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="M23:O23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="M27:O27"/>
-    <mergeCell ref="E28:H28"/>
     <mergeCell ref="J28:L28"/>
     <mergeCell ref="M28:O28"/>
     <mergeCell ref="J29:L29"/>
     <mergeCell ref="M29:O29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K31:M31"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.0" footer="0.0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>